<commit_message>
added occupancy type to Cyprus mapping
</commit_message>
<xml_diff>
--- a/res_mapping_schemes/mapping_Cyprus_RES.xlsx
+++ b/res_mapping_schemes/mapping_Cyprus_RES.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11111"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{705C146A-2A72-CF4D-B2CF-4840C7FB3D33}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF2B8652-8BA9-FF4B-A902-3C5FE826F943}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="22260" windowHeight="12640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="22260" windowHeight="12640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mapping_urban" sheetId="1" r:id="rId1"/>
@@ -44,141 +44,148 @@
     <t>Other type of building</t>
   </si>
   <si>
-    <t xml:space="preserve">3% CR/LFINF+CDM/H:1 
-3% CR/LFINF+CDN/H:1 
-21% CR/LFINF+CDM/H:2 
-40% CR/LFINF+CDN/H:2 
-5% CR/LFINF+CDN/H:2/SOS 
-10% CR/LFINF+CDN/H:2/SOS 
-4% CR/LDUAL+CDN/H:2/SOS 
-6% MUR/LWAL+CDN/H:1 
-5% MUR/LWAL+CDN/H:2 
-3% MUR+ADO/LWAL+CDN/H:1 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">47% CR/LFINF+CDM/H:2 
-20% CR/LFINF+CDN/H:2 
-7% CR/LFINF+CDN/H:2/SOS 
-5% CR/LFINF+CDN/H:2/SOS 
-3% CR/LFINF+CDN/HBET:3-5 
-1% CR/LFINF+CDN/HBET:3-5/SOS 
-3% CR/LDUAL+CDN/H:2/SOS 
-1% CR/LDUAL+CDN/HBET:3-5/SOS 
-10% MUR/LWAL+CDN/H:2 
-3% MUR+ADO/LWAL+CDN/H:1 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">3% CR/LFINF+CDM/H:1 
-3% CR/LFINF+CDN/H:1 
-25% CR/LFINF+CDM/H:2 
-25% CR/LFINF+CDN/H:2 
-7% CR/LFINF+CDN/H:2/SOS 
-5% CR/LFINF+CDN/H:2/SOS 
-13% CR/LFINF+CDM/HBET:3-5 
-1% CR/LFINF+CDN/HBET:3-5/SOS 
-3% CR/LDUAL+CDN/H:2/SOS 
-1% CR/LDUAL+CDN/HBET:3-5/SOS 
-6% MUR/LWAL+CDN/H:1 
-5% MUR/LWAL+CDN/H:2 
-3% MUR+ADO/LWAL+CDN/H:1 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">3% CR/LFINF+CDM/H:1 
-3% CR/LFINF+CDN/H:1 
-30% CR/LFINF+CDM/H:2 
-25% CR/LFINF+CDN/H:2 
-7% CR/LFINF+CDN/H:2/SOS 
-5% CR/LFINF+CDN/H:2/SOS 
-8% CR/LFINF+CDM/HBET:3-5 
-1% CR/LFINF+CDN/HBET:3-5/SOS 
-3% CR/LDUAL+CDN/H:2/SOS 
-1% CR/LDUAL+CDN/HBET:3-5/SOS 
-6% MUR/LWAL+CDN/H:1 
-5% MUR/LWAL+CDN/H:2 
-3% MUR+ADO/LWAL+CDN/H:1 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">3% CR/LFINF+CDN/H:1 
-3% CR/LFINF+CDN/H:1 
-35% CR/LFINF+CDN/H:2 
-25% CR/LFINF+CDN/H:2 
-7% CR/LFINF+CDN/H:2/SOS 
-5% CR/LFINF+CDN/H:2/SOS 
-3% CR/LFINF+CDN/HBET:3-5 
-1% CR/LFINF+CDN/HBET:3-5/SOS 
-3% CR/LDUAL+CDN/H:2/SOS 
-1% CR/LDUAL+CDN/HBET:3-5/SOS 
-6% MUR/LWAL+CDN/H:1 
-5% MUR/LWAL+CDN/H:2 
-3% MUR+ADO/LWAL+CDN/H:1 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">25% CR/LFINF+CDM/H:2 
-25% CR/LFINF+CDN/H:2 
-7% CR/LFINF+CDN/H:2/SOS 
-4% CR/LFINF+CDM/HBET:3-5 
-10% CR/LFINF+CDM/HBET:6- 
-1% CR/LFINF+CDN/HBET:3-5/SOS 
-8% CR/LDUAL+CDN/H:2/SOS 
-15% CR/LDUAL+CDN/HBET:3-5/SOS 
-5% MUR/LWAL+CDN/H:2 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">5% CR/LFINF+CDM/H:1 
-20% CR/LFINF+CDM/H:2 
-10% CR/LFINF+CDM/HBET:6- 
-32% CR/LFINF+CDN/H:2 
-8% CR/LFINF+CDN/H:2/SOS 
-4% CR/LFINF+CDN/H:2/SOS 
-3% CR/LFINF+CDM/HBET:3-5 
-1% CR/LFINF+CDN/HBET:6-/SOS 
-3% CR/LDUAL+CDN/H:2/SOS 
-4% CR/LDUAL+CDN/HBET:3-5/SOS 
-5% MUR/LWAL+CDN/H:1 
-5% MUR/LWAL+CDN/H:2 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">20% CR/LFINF+CDN/H:2 
-20% CR/LFINF+CDN/H:2 
-35% CR/LFINF+CDN/HBET:3-5 
-20% CR/LFINF+CDN/HBET:3-5 
-5% MUR/LWAL+CDN/H:2 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">35% CR/LFINF+CDN/H:1 
-10% CR/LFINF+CDN/H:2 
-5% CR/LFINF+CDN/HBET:3-5/SOS 
-45% MUR/LWAL+CDN/H:1 
-5% MUR/LWAL+CDN/H:2 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">45% CR/LFINF+CDN/H:1 
-5% CR/LFINF+CDN/H:2 
-50% MUR/LWAL+CDN/H:1 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">45% CR/LFINF+CDN/H:2 
-5% CR/LFINF+CDN/HBET:3-5 
-50% MUR/LWAL+CDN/H:2 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">35% CR/LFINF+CDN/H:1 
-10% CR/LFINF+CDN/H:2 
-5% CR/LFINF+CDN/HBET:3-5 
-45% MUR/LWAL+CDN/H:1 
-5% MUR/LWAL+CDN/H:2 </t>
-  </si>
-  <si>
     <t>Dwelling type</t>
+  </si>
+  <si>
+    <t>3% CR/LFINF+CDM/H:1/Single
+3% CR/LFINF+CDN/H:1/Single
+21% CR/LFINF+CDM/H:2/Single
+40% CR/LFINF+CDN/H:2/Single
+5% CR/LFINF+CDN/H:2/SOS/Single
+10% CR/LFINF+CDN/H:2/SOS/Single
+4% CR/LDUAL+CDN/H:2/SOS/Single
+6% MUR/LWAL+CDN/H:1/Single
+5% MUR/LWAL+CDN/H:2/Single
+3% MUR+ADO/LWAL+CDN/H:1/Single</t>
+  </si>
+  <si>
+    <t>47% CR/LFINF+CDM/H:2/Single
+20% CR/LFINF+CDN/H:2/Single
+7% CR/LFINF+CDN/H:2/SOS/Single
+5% CR/LFINF+CDN/H:2/SOS/Single
+3% CR/LFINF+CDN/HBET:3-5/Single
+1% CR/LFINF+CDN/HBET:3-5/SOS/Single
+3% CR/LDUAL+CDN/H:2/SOS/Single
+1% CR/LDUAL+CDN/HBET:3-5/SOS/Single
+10% MUR/LWAL+CDN/H:2/Single
+3% MUR+ADO/LWAL+CDN/H:1/Single</t>
+  </si>
+  <si>
+    <t>3% CR/LFINF+CDM/H:1/Single
+3% CR/LFINF+CDN/H:1/Single
+25% CR/LFINF+CDM/H:2/Single
+25% CR/LFINF+CDN/H:2/Single
+7% CR/LFINF+CDN/H:2/SOS/Single
+5% CR/LFINF+CDN/H:2/SOS/Single
+13% CR/LFINF+CDM/HBET:3-5/Single
+1% CR/LFINF+CDN/HBET:3-5/SOS/Single
+3% CR/LDUAL+CDN/H:2/SOS/Single
+1% CR/LDUAL+CDN/HBET:3-5/SOS/Single
+6% MUR/LWAL+CDN/H:1/Single
+5% MUR/LWAL+CDN/H:2/Single
+3% MUR+ADO/LWAL+CDN/H:1/Single</t>
+  </si>
+  <si>
+    <t>3% CR/LFINF+CDM/H:1/Single
+3% CR/LFINF+CDN/H:1/Single
+30% CR/LFINF+CDM/H:2/Single
+25% CR/LFINF+CDN/H:2/Single
+7% CR/LFINF+CDN/H:2/SOS/Single
+5% CR/LFINF+CDN/H:2/SOS/Single
+8% CR/LFINF+CDM/HBET:3-5/Single
+1% CR/LFINF+CDN/HBET:3-5/SOS/Single
+3% CR/LDUAL+CDN/H:2/SOS/Single
+1% CR/LDUAL+CDN/HBET:3-5/SOS/Single
+6% MUR/LWAL+CDN/H:1/Single
+5% MUR/LWAL+CDN/H:2/Single
+3% MUR+ADO/LWAL+CDN/H:1/Single</t>
+  </si>
+  <si>
+    <t>25% CR/LFINF+CDM/H:2/Apartment
+25% CR/LFINF+CDN/H:2/Apartment
+7% CR/LFINF+CDN/H:2/SOS/Apartment
+4% CR/LFINF+CDM/HBET:3-5/Apartment
+10% CR/LFINF+CDM/HBET:6-/Apartment
+1% CR/LFINF+CDN/HBET:3-5/SOS/Apartment
+8% CR/LDUAL+CDN/H:2/SOS/Apartment
+15% CR/LDUAL+CDN/HBET:3-5/SOS/Apartment
+5% MUR/LWAL+CDN/H:2/Apartment</t>
+  </si>
+  <si>
+    <t>5% CR/LFINF+CDM/H:1/Apartment
+20% CR/LFINF+CDM/H:2/Apartment
+10% CR/LFINF+CDM/HBET:6-/Apartment
+32% CR/LFINF+CDN/H:2/Apartment
+8% CR/LFINF+CDN/H:2/SOS/Apartment
+4% CR/LFINF+CDN/H:2/SOS/Apartment
+3% CR/LFINF+CDM/HBET:3-5/Apartment
+1% CR/LFINF+CDN/HBET:6-/SOS/Apartment
+3% CR/LDUAL+CDN/H:2/SOS/Apartment
+4% CR/LDUAL+CDN/HBET:3-5/SOS/Apartment
+5% MUR/LWAL+CDN/H:1/Apartment
+5% MUR/LWAL+CDN/H:2/Apartment</t>
+  </si>
+  <si>
+    <t>3% CR/LFINF+CDN/H:1/Single
+3% CR/LFINF+CDN/H:1/Single
+35% CR/LFINF+CDN/H:2/Single
+25% CR/LFINF+CDN/H:2/Single
+7% CR/LFINF+CDN/H:2/SOS/Single
+5% CR/LFINF+CDN/H:2/SOS/Single
+3% CR/LFINF+CDN/HBET:3-5/Single
+1% CR/LFINF+CDN/HBET:3-5/SOS/Single
+3% CR/LDUAL+CDN/H:2/SOS/Single
+1% CR/LDUAL+CDN/HBET:3-5/SOS/Single
+6% MUR/LWAL+CDN/H:1/Single
+5% MUR/LWAL+CDN/H:2/Single
+3% MUR+ADO/LWAL+CDN/H:1/Single</t>
+  </si>
+  <si>
+    <t>45% CR/LFINF+CDN/H:1/Single
+5% CR/LFINF+CDN/H:2/Single
+50% MUR/LWAL+CDN/H:1/Single</t>
+  </si>
+  <si>
+    <t>45% CR/LFINF+CDN/H:2/Single
+5% CR/LFINF+CDN/HBET:3-5/Single
+50% MUR/LWAL+CDN/H:2/Single</t>
+  </si>
+  <si>
+    <t>35% CR/LFINF+CDN/H:1/Single
+10% CR/LFINF+CDN/H:2/Single
+5% CR/LFINF+CDN/HBET:3-5/Single
+45% MUR/LWAL+CDN/H:1/Single
+5% MUR/LWAL+CDN/H:2/Single</t>
+  </si>
+  <si>
+    <t>20% CR/LFINF+CDN/H:2/Apartment
+20% CR/LFINF+CDN/H:2/Apartment
+35% CR/LFINF+CDN/HBET:3-5/Apartment
+20% CR/LFINF+CDN/HBET:3-5/Apartment
+5% MUR/LWAL+CDN/H:2/Apartment</t>
+  </si>
+  <si>
+    <t>35% CR/LFINF+CDN/H:1/Apartment
+10% CR/LFINF+CDN/H:2/Apartment
+5% CR/LFINF+CDN/HBET:3-5/SOS/Apartment
+45% MUR/LWAL+CDN/H:1/Apartment
+5% MUR/LWAL+CDN/H:2/Apartment</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -247,18 +254,18 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -543,8 +550,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -560,53 +567,53 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="95.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B1" s="2" t="s">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="219" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3"/>
-      <c r="B2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="A2" s="2"/>
+      <c r="B2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="C2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="D2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="E2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>11</v>
+      <c r="H2" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -618,8 +625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -627,7 +634,7 @@
     <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.1640625" customWidth="1"/>
     <col min="3" max="3" width="33" customWidth="1"/>
-    <col min="4" max="4" width="30" customWidth="1"/>
+    <col min="4" max="4" width="32.83203125" customWidth="1"/>
     <col min="5" max="5" width="31.5" customWidth="1"/>
     <col min="6" max="6" width="39.83203125" customWidth="1"/>
     <col min="7" max="7" width="46" customWidth="1"/>
@@ -635,53 +642,53 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="100.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="102" x14ac:dyDescent="0.2">
+      <c r="A2" s="2"/>
+      <c r="B2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="85" x14ac:dyDescent="0.2">
-      <c r="A2" s="3"/>
-      <c r="B2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="H2" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>